<commit_message>
Update DLC chapter overview (id, name, rDate, category, dlcCategories, release, codeName, Folder, Characters).xlsx
</commit_message>
<xml_diff>
--- a/Program/Assets/DLC chapter overview (id, name, rDate, category, dlcCategories, release, codeName, Folder, Characters).xlsx
+++ b/Program/Assets/DLC chapter overview (id, name, rDate, category, dlcCategories, release, codeName, Folder, Characters).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Perk-Randomiser-for-Dead-by-Daylight\Program\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7508A5-4DDB-4A95-97D7-9990729A01A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664F93B3-6074-49E9-8F7C-2099B2A6BC3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12345" yWindow="3435" windowWidth="21540" windowHeight="15105" xr2:uid="{898976F4-4C52-43AD-8236-3E3A81667028}"/>
+    <workbookView xWindow="36240" yWindow="4020" windowWidth="21540" windowHeight="15105" xr2:uid="{898976F4-4C52-43AD-8236-3E3A81667028}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -719,12 +719,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -739,9 +745,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1078,8 +1085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7EA9D9E-7D72-475F-A94B-28D996D3C3C2}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1135,7 +1142,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="str">
-        <f>CHOOSE(D2, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" ref="E2:E43" si="0">CHOOSE(D2, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
         <v>Chapter DLC</v>
       </c>
       <c r="F2" t="s">
@@ -1151,33 +1158,33 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="str">
-        <f>CHOOSE(D3, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
-        <v>Chapter DLC</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Chapter DLC</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="H3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="H3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>180</v>
       </c>
     </row>
@@ -1195,7 +1202,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="str">
-        <f>CHOOSE(D4, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F4" t="s">
@@ -1225,7 +1232,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="str">
-        <f>CHOOSE(D5, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F5" t="s">
@@ -1255,7 +1262,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="str">
-        <f>CHOOSE(D6, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F6" t="s">
@@ -1285,7 +1292,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="str">
-        <f>CHOOSE(D7, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F7" t="s">
@@ -1316,7 +1323,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="str">
-        <f>CHOOSE(D8, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F8" t="s">
@@ -1347,7 +1354,7 @@
         <v>1</v>
       </c>
       <c r="E9" t="str">
-        <f>CHOOSE(D9, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F9" t="s">
@@ -1377,7 +1384,7 @@
         <v>1</v>
       </c>
       <c r="E10" t="str">
-        <f>CHOOSE(D10, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F10" t="s">
@@ -1387,7 +1394,7 @@
         <v>50</v>
       </c>
       <c r="H10" t="str">
-        <f>G10</f>
+        <f t="shared" ref="H10:H17" si="1">G10</f>
         <v>Guam</v>
       </c>
       <c r="I10" t="s">
@@ -1408,7 +1415,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="str">
-        <f>CHOOSE(D11, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F11" t="s">
@@ -1418,7 +1425,7 @@
         <v>48</v>
       </c>
       <c r="H11" t="str">
-        <f>G11</f>
+        <f t="shared" si="1"/>
         <v>Haiti</v>
       </c>
       <c r="I11" t="s">
@@ -1439,7 +1446,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="str">
-        <f>CHOOSE(D12, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F12" t="s">
@@ -1449,7 +1456,7 @@
         <v>42</v>
       </c>
       <c r="H12" t="str">
-        <f>G12</f>
+        <f t="shared" si="1"/>
         <v>Kenya</v>
       </c>
       <c r="I12" t="s">
@@ -1470,7 +1477,7 @@
         <v>1</v>
       </c>
       <c r="E13" t="str">
-        <f>CHOOSE(D13, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F13" t="s">
@@ -1480,7 +1487,7 @@
         <v>38</v>
       </c>
       <c r="H13" t="str">
-        <f>G13</f>
+        <f t="shared" si="1"/>
         <v>Mali</v>
       </c>
       <c r="I13" t="s">
@@ -1501,7 +1508,7 @@
         <v>1</v>
       </c>
       <c r="E14" t="str">
-        <f>CHOOSE(D14, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F14" t="s">
@@ -1511,7 +1518,7 @@
         <v>34</v>
       </c>
       <c r="H14" t="str">
-        <f>G14</f>
+        <f t="shared" si="1"/>
         <v>Oman</v>
       </c>
       <c r="I14" t="s">
@@ -1532,7 +1539,7 @@
         <v>1</v>
       </c>
       <c r="E15" t="str">
-        <f>CHOOSE(D15, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F15" t="s">
@@ -1542,7 +1549,7 @@
         <v>30</v>
       </c>
       <c r="H15" t="str">
-        <f>G15</f>
+        <f t="shared" si="1"/>
         <v>Qatar</v>
       </c>
       <c r="I15" t="s">
@@ -1563,7 +1570,7 @@
         <v>1</v>
       </c>
       <c r="E16" t="str">
-        <f>CHOOSE(D16, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F16" t="s">
@@ -1573,7 +1580,7 @@
         <v>24</v>
       </c>
       <c r="H16" t="str">
-        <f>G16</f>
+        <f t="shared" si="1"/>
         <v>Sweden</v>
       </c>
       <c r="I16" t="s">
@@ -1594,7 +1601,7 @@
         <v>1</v>
       </c>
       <c r="E17" t="str">
-        <f>CHOOSE(D17, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F17" t="s">
@@ -1604,7 +1611,7 @@
         <v>22</v>
       </c>
       <c r="H17" t="str">
-        <f>G17</f>
+        <f t="shared" si="1"/>
         <v>Ukraine</v>
       </c>
       <c r="I17" t="s">
@@ -1625,7 +1632,7 @@
         <v>2</v>
       </c>
       <c r="E18" t="str">
-        <f>CHOOSE(D18, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Half-Chapter DLC</v>
       </c>
       <c r="F18" t="s">
@@ -1655,7 +1662,7 @@
         <v>2</v>
       </c>
       <c r="E19" t="str">
-        <f>CHOOSE(D19, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Half-Chapter DLC</v>
       </c>
       <c r="F19" t="s">
@@ -1685,7 +1692,7 @@
         <v>2</v>
       </c>
       <c r="E20" t="str">
-        <f>CHOOSE(D20, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Half-Chapter DLC</v>
       </c>
       <c r="F20" t="s">
@@ -1715,7 +1722,7 @@
         <v>1</v>
       </c>
       <c r="E21" t="str">
-        <f>CHOOSE(D21, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F21" t="s">
@@ -1725,7 +1732,7 @@
         <v>16</v>
       </c>
       <c r="H21" t="str">
-        <f>G21</f>
+        <f t="shared" ref="H21:H44" si="2">G21</f>
         <v>Wales</v>
       </c>
       <c r="I21" t="s">
@@ -1746,7 +1753,7 @@
         <v>1</v>
       </c>
       <c r="E22" t="str">
-        <f>CHOOSE(D22, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F22" t="s">
@@ -1756,7 +1763,7 @@
         <v>12</v>
       </c>
       <c r="H22" t="str">
-        <f>G22</f>
+        <f t="shared" si="2"/>
         <v>Yemen</v>
       </c>
       <c r="I22" t="s">
@@ -1777,7 +1784,7 @@
         <v>1</v>
       </c>
       <c r="E23" t="str">
-        <f>CHOOSE(D23, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F23" t="s">
@@ -1787,7 +1794,7 @@
         <v>70</v>
       </c>
       <c r="H23" t="str">
-        <f>G23</f>
+        <f t="shared" si="2"/>
         <v>Aurora</v>
       </c>
       <c r="I23" t="s">
@@ -1808,7 +1815,7 @@
         <v>1</v>
       </c>
       <c r="E24" t="str">
-        <f>CHOOSE(D24, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F24" t="s">
@@ -1818,7 +1825,7 @@
         <v>66</v>
       </c>
       <c r="H24" t="str">
-        <f>G24</f>
+        <f t="shared" si="2"/>
         <v>Comet</v>
       </c>
       <c r="I24" t="s">
@@ -1839,7 +1846,7 @@
         <v>1</v>
       </c>
       <c r="E25" t="str">
-        <f>CHOOSE(D25, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F25" t="s">
@@ -1849,7 +1856,7 @@
         <v>60</v>
       </c>
       <c r="H25" t="str">
-        <f>G25</f>
+        <f t="shared" si="2"/>
         <v>Eclipse</v>
       </c>
       <c r="I25" t="s">
@@ -1870,7 +1877,7 @@
         <v>1</v>
       </c>
       <c r="E26" t="str">
-        <f>CHOOSE(D26, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F26" t="s">
@@ -1880,7 +1887,7 @@
         <v>52</v>
       </c>
       <c r="H26" t="str">
-        <f>G26</f>
+        <f t="shared" si="2"/>
         <v>Gemini</v>
       </c>
       <c r="I26" t="s">
@@ -1901,7 +1908,7 @@
         <v>2</v>
       </c>
       <c r="E27" t="str">
-        <f>CHOOSE(D27, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Half-Chapter DLC</v>
       </c>
       <c r="F27" t="s">
@@ -1911,7 +1918,7 @@
         <v>46</v>
       </c>
       <c r="H27" t="str">
-        <f>G27</f>
+        <f t="shared" si="2"/>
         <v>Hubble</v>
       </c>
       <c r="I27" t="s">
@@ -1932,7 +1939,7 @@
         <v>1</v>
       </c>
       <c r="E28" t="str">
-        <f>CHOOSE(D28, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F28" t="s">
@@ -1942,7 +1949,7 @@
         <v>44</v>
       </c>
       <c r="H28" t="str">
-        <f>G28</f>
+        <f t="shared" si="2"/>
         <v>Ion</v>
       </c>
       <c r="I28" t="s">
@@ -1963,7 +1970,7 @@
         <v>1</v>
       </c>
       <c r="E29" t="str">
-        <f>CHOOSE(D29, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F29" t="s">
@@ -1973,7 +1980,7 @@
         <v>40</v>
       </c>
       <c r="H29" t="str">
-        <f>G29</f>
+        <f t="shared" si="2"/>
         <v>Kepler</v>
       </c>
       <c r="I29" t="s">
@@ -1994,7 +2001,7 @@
         <v>1</v>
       </c>
       <c r="E30" t="str">
-        <f>CHOOSE(D30, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F30" t="s">
@@ -2004,7 +2011,7 @@
         <v>36</v>
       </c>
       <c r="H30" t="str">
-        <f>G30</f>
+        <f t="shared" si="2"/>
         <v>Meteor</v>
       </c>
       <c r="I30" t="s">
@@ -2025,7 +2032,7 @@
         <v>1</v>
       </c>
       <c r="E31" t="str">
-        <f>CHOOSE(D31, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F31" t="s">
@@ -2035,7 +2042,7 @@
         <v>32</v>
       </c>
       <c r="H31" t="str">
-        <f>G31</f>
+        <f t="shared" si="2"/>
         <v>Orion</v>
       </c>
       <c r="I31" t="s">
@@ -2056,7 +2063,7 @@
         <v>1</v>
       </c>
       <c r="E32" t="str">
-        <f>CHOOSE(D32, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F32" t="s">
@@ -2066,7 +2073,7 @@
         <v>28</v>
       </c>
       <c r="H32" t="str">
-        <f>G32</f>
+        <f t="shared" si="2"/>
         <v>Quantum</v>
       </c>
       <c r="I32" t="s">
@@ -2087,7 +2094,7 @@
         <v>1</v>
       </c>
       <c r="E33" t="str">
-        <f>CHOOSE(D33, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F33" t="s">
@@ -2097,7 +2104,7 @@
         <v>26</v>
       </c>
       <c r="H33" t="str">
-        <f>G33</f>
+        <f t="shared" si="2"/>
         <v>Saturn</v>
       </c>
       <c r="I33" t="s">
@@ -2118,7 +2125,7 @@
         <v>1</v>
       </c>
       <c r="E34" t="str">
-        <f>CHOOSE(D34, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F34" t="s">
@@ -2128,7 +2135,7 @@
         <v>20</v>
       </c>
       <c r="H34" t="str">
-        <f>G34</f>
+        <f t="shared" si="2"/>
         <v>Umbra</v>
       </c>
       <c r="I34" t="s">
@@ -2149,7 +2156,7 @@
         <v>2</v>
       </c>
       <c r="E35" t="str">
-        <f>CHOOSE(D35, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Half-Chapter DLC</v>
       </c>
       <c r="F35" t="s">
@@ -2159,7 +2166,7 @@
         <v>18</v>
       </c>
       <c r="H35" t="str">
-        <f>G35</f>
+        <f t="shared" si="2"/>
         <v>Venus</v>
       </c>
       <c r="I35" t="s">
@@ -2180,7 +2187,7 @@
         <v>1</v>
       </c>
       <c r="E36" t="str">
-        <f>CHOOSE(D36, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F36" t="s">
@@ -2190,7 +2197,7 @@
         <v>14</v>
       </c>
       <c r="H36" t="str">
-        <f>G36</f>
+        <f t="shared" si="2"/>
         <v>Wormhole</v>
       </c>
       <c r="I36" t="s">
@@ -2211,7 +2218,7 @@
         <v>1</v>
       </c>
       <c r="E37" t="str">
-        <f>CHOOSE(D37, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F37" t="s">
@@ -2221,7 +2228,7 @@
         <v>11</v>
       </c>
       <c r="H37" t="str">
-        <f>G37</f>
+        <f t="shared" si="2"/>
         <v>Yerkes</v>
       </c>
       <c r="I37" t="s">
@@ -2242,7 +2249,7 @@
         <v>2</v>
       </c>
       <c r="E38" t="str">
-        <f>CHOOSE(D38, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Half-Chapter DLC</v>
       </c>
       <c r="F38" t="s">
@@ -2252,7 +2259,7 @@
         <v>9</v>
       </c>
       <c r="H38" t="str">
-        <f>G38</f>
+        <f t="shared" si="2"/>
         <v>Zodiac</v>
       </c>
       <c r="I38" t="s">
@@ -2273,7 +2280,7 @@
         <v>1</v>
       </c>
       <c r="E39" t="str">
-        <f>CHOOSE(D39, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F39" t="s">
@@ -2283,7 +2290,7 @@
         <v>83</v>
       </c>
       <c r="H39" t="str">
-        <f>G39</f>
+        <f t="shared" si="2"/>
         <v>ApplePie</v>
       </c>
       <c r="I39" t="s">
@@ -2304,7 +2311,7 @@
         <v>1</v>
       </c>
       <c r="E40" t="str">
-        <f>CHOOSE(D40, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F40" t="s">
@@ -2314,7 +2321,7 @@
         <v>68</v>
       </c>
       <c r="H40" t="str">
-        <f>G40</f>
+        <f t="shared" si="2"/>
         <v>Churros</v>
       </c>
       <c r="I40" t="s">
@@ -2335,7 +2342,7 @@
         <v>2</v>
       </c>
       <c r="E41" t="str">
-        <f>CHOOSE(D41, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Half-Chapter DLC</v>
       </c>
       <c r="F41" t="s">
@@ -2345,7 +2352,7 @@
         <v>64</v>
       </c>
       <c r="H41" t="str">
-        <f>G41</f>
+        <f t="shared" si="2"/>
         <v>Donut</v>
       </c>
       <c r="I41" t="s">
@@ -2366,7 +2373,7 @@
         <v>1</v>
       </c>
       <c r="E42" t="str">
-        <f>CHOOSE(D42, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F42" t="s">
@@ -2376,7 +2383,7 @@
         <v>62</v>
       </c>
       <c r="H42" t="str">
-        <f>G42</f>
+        <f t="shared" si="2"/>
         <v>Éclair</v>
       </c>
       <c r="I42" t="s">
@@ -2397,7 +2404,7 @@
         <v>1</v>
       </c>
       <c r="E43" t="str">
-        <f>CHOOSE(D43, "Chapter DLC", "Half-Chapter DLC", "Clothing Pack DLC", "Original Soundtrack DLC", "Character Pack DLC", "Other", "Retracted", "Chapter Pack DLC")</f>
+        <f t="shared" si="0"/>
         <v>Chapter DLC</v>
       </c>
       <c r="F43" t="s">
@@ -2407,7 +2414,7 @@
         <v>54</v>
       </c>
       <c r="H43" t="str">
-        <f>G43</f>
+        <f t="shared" si="2"/>
         <v>Gelato</v>
       </c>
       <c r="I43" t="s">
@@ -2415,6 +2422,9 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>56</v>
+      </c>
       <c r="B44" t="s">
         <v>173</v>
       </c>
@@ -2422,7 +2432,7 @@
         <v>174</v>
       </c>
       <c r="H44" t="str">
-        <f>G44</f>
+        <f t="shared" si="2"/>
         <v>Icecream</v>
       </c>
       <c r="I44" t="s">

</xml_diff>